<commit_message>
Dev: Create service discovery for fetch category.
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC66B9B-8998-C146-BC08-63C705EC5955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337644CF-33E2-1640-8F49-01F4405B5AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>service-name</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t xml:space="preserve"> /selling/source/sale/v1/</t>
+  </si>
+  <si>
+    <t>fetch-eureka-server</t>
+  </si>
+  <si>
+    <t>reports-eureka-server</t>
+  </si>
+  <si>
+    <t>persistence-eureka-server</t>
   </si>
 </sst>
 </file>
@@ -507,16 +516,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="244" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -578,58 +587,94 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4">
-        <v>6013</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8000</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6013</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>6014</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8001</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C9" s="5">
         <v>6015</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5">
+        <v>8002</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C11" s="1">
         <v>6016</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dev: Finish Eureka server and clients for reports catalog.
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337644CF-33E2-1640-8F49-01F4405B5AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5FCF68-315A-6F49-867B-13DD8BEE5A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20120" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>service-name</t>
   </si>
@@ -68,18 +68,12 @@
     <t>fetch-stores-ms</t>
   </si>
   <si>
-    <t>/selling/generate/sale/report/v1/</t>
-  </si>
-  <si>
     <t>reports</t>
   </si>
   <si>
     <t>receipt-generator-ms</t>
   </si>
   <si>
-    <t>/selling/calc/price/v1/</t>
-  </si>
-  <si>
     <t>calc-price-ms</t>
   </si>
   <si>
@@ -111,6 +105,18 @@
   </si>
   <si>
     <t>persistence-eureka-server</t>
+  </si>
+  <si>
+    <t>/selling/fetch/</t>
+  </si>
+  <si>
+    <t>/selling/reports/generate/sale/v1/</t>
+  </si>
+  <si>
+    <t>/selling/reports/calc/price/v1/</t>
+  </si>
+  <si>
+    <t>/selling/reports/</t>
   </si>
 </sst>
 </file>
@@ -519,7 +525,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="244" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -591,73 +597,77 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3">
         <v>8000</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C6" s="4">
         <v>6013</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4">
         <v>6014</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
         <v>8001</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5">
         <v>6015</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5">
         <v>8002</v>
@@ -666,16 +676,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1">
         <v>6016</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dev: start working on export module and finish data-export-json service.
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADDF883-BE06-B84C-AC92-E00671F8FCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC58B137-AD25-7D40-A04C-AC296542D56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
   <si>
     <t>service-name</t>
   </si>
@@ -333,6 +333,39 @@
   </si>
   <si>
     <t>sales-pull-ms</t>
+  </si>
+  <si>
+    <t>export-data-pdf</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>export-data-csv</t>
+  </si>
+  <si>
+    <t>export-data-excel</t>
+  </si>
+  <si>
+    <t>export-data-json</t>
+  </si>
+  <si>
+    <t>export-data-xml</t>
+  </si>
+  <si>
+    <t>/selling/export/sales/pdf/</t>
+  </si>
+  <si>
+    <t>/selling/export/sales/csv/</t>
+  </si>
+  <si>
+    <t>/selling/export/sales/excel/</t>
+  </si>
+  <si>
+    <t>/selling/export/sales/json/</t>
+  </si>
+  <si>
+    <t>/selling/export/sales/xml/</t>
   </si>
 </sst>
 </file>
@@ -765,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1544,6 +1577,91 @@
         <v>96</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>48</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="3">
+        <v>7030</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>49</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="3">
+        <v>7031</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>50</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="3">
+        <v>7032</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>51</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="3">
+        <v>7033</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>52</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="3">
+        <v>7034</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add the background to the archi picture
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22AE528-8F65-BB47-A8BA-99312DEFFD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AE0DA2-86D5-8C4C-B8D2-1D7CBE71690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -801,7 +801,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Dev: Complete export category
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AE0DA2-86D5-8C4C-B8D2-1D7CBE71690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FEACBB-8A79-A242-9658-34627E7175AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
     <t>service-name</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>export-data-xlsx</t>
+  </si>
+  <si>
+    <t>export-data-manager-ms</t>
+  </si>
+  <si>
+    <t>/selling/export/sales/manager/</t>
   </si>
 </sst>
 </file>
@@ -798,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,70 +1516,70 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+      <c r="A42" s="1">
         <v>44</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="1">
         <v>7020</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+      <c r="A43" s="1">
         <v>45</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="1">
         <v>7021</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+      <c r="A44" s="1">
         <v>46</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="1">
         <v>7022</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+      <c r="A45" s="1">
         <v>47</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="1">
         <v>7023</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="1" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1660,6 +1666,23 @@
       </c>
       <c r="E50" s="3" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>53</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="3">
+        <v>7035</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dev: Creates initial structure of auth category
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FEACBB-8A79-A242-9658-34627E7175AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4A4B3B-4B99-6D40-A4E8-63A130D84FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
   <si>
     <t>service-name</t>
   </si>
@@ -372,6 +372,27 @@
   </si>
   <si>
     <t>/selling/export/sales/manager/</t>
+  </si>
+  <si>
+    <t>auth</t>
+  </si>
+  <si>
+    <t>auth-manager</t>
+  </si>
+  <si>
+    <t>/selling/auth/manager/</t>
+  </si>
+  <si>
+    <t>auth-users-manager</t>
+  </si>
+  <si>
+    <t>auth-profiles-manager</t>
+  </si>
+  <si>
+    <t>/selling/auth/users/manager/</t>
+  </si>
+  <si>
+    <t>/selling/auth/profiles/manager/</t>
   </si>
 </sst>
 </file>
@@ -804,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,6 +1706,57 @@
         <v>111</v>
       </c>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>54</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="5">
+        <v>7040</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>55</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="5">
+        <v>7041</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>56</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="5">
+        <v>7042</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dev: Handle reading resource bundles and switch between different locals based on a header parameter and link them to the exception advisor.
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4A4B3B-4B99-6D40-A4E8-63A130D84FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E720F3-E0A5-B745-8756-33C3ABAC8977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -828,7 +828,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DEV: create a new service and move some folders,modify .gitignore
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E720F3-E0A5-B745-8756-33C3ABAC8977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B45D5E2-A974-6546-AD95-1466678A250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="121">
   <si>
     <t>service-name</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>/selling/auth/profiles/manager/</t>
+  </si>
+  <si>
+    <t>auth-clients-manager</t>
+  </si>
+  <si>
+    <t>/selling/auth/clients/manager/</t>
   </si>
 </sst>
 </file>
@@ -825,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1757,6 +1763,23 @@
         <v>118</v>
       </c>
     </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>57</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="5">
+        <v>7043</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dev: Implement PKCE grant type.
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B45D5E2-A974-6546-AD95-1466678A250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07A1239-3D10-3343-A77F-77079D6A9759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>service-name</t>
   </si>
@@ -399,6 +399,36 @@
   </si>
   <si>
     <t>/selling/auth/clients/manager/</t>
+  </si>
+  <si>
+    <t>redis</t>
+  </si>
+  <si>
+    <t>redis-node1</t>
+  </si>
+  <si>
+    <t>redis-node2</t>
+  </si>
+  <si>
+    <t>redis-node3</t>
+  </si>
+  <si>
+    <t>redis-node4</t>
+  </si>
+  <si>
+    <t>redis-node5</t>
+  </si>
+  <si>
+    <t>redis-node6</t>
+  </si>
+  <si>
+    <t>redis-cluster-creator</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>redis-insight</t>
   </si>
 </sst>
 </file>
@@ -414,7 +444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +493,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -491,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -515,6 +551,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -831,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,6 +1819,142 @@
         <v>120</v>
       </c>
     </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="9">
+        <v>58</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" s="9">
+        <v>7050</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="9">
+        <v>59</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D57" s="9">
+        <v>7051</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="9">
+        <v>60</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" s="9">
+        <v>7052</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="9">
+        <v>61</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D59" s="9">
+        <v>7053</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="9">
+        <v>62</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="9">
+        <v>7054</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="9">
+        <v>63</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="9">
+        <v>7055</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="9">
+        <v>64</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="9">
+        <v>7056</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="9">
+        <v>65</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D63" s="9">
+        <v>7057</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dev: Dockerize the data category in more elegant way
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07A1239-3D10-3343-A77F-77079D6A9759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49039AF3-8F07-B447-B9BA-B00FFA3502CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DEV: Fix issues in data/get category while retriveing data in docker
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49039AF3-8F07-B447-B9BA-B00FFA3502CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E430637-9429-3F4A-BE16-82C34CF76E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D46" sqref="C46:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1957,5 +1957,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DEV: Finish refactoring data-save-order service
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E430637-9429-3F4A-BE16-82C34CF76E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF3705C-686F-4E43-86FB-FD48A47E4F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -77,12 +77,6 @@
     <t xml:space="preserve"> /selling/source/push/sale/v1/</t>
   </si>
   <si>
-    <t>sales-get-ms</t>
-  </si>
-  <si>
-    <t>sales-save-ms</t>
-  </si>
-  <si>
     <t>sales-delete-ms</t>
   </si>
   <si>
@@ -209,12 +203,6 @@
     <t>search-sales-manager-ms</t>
   </si>
   <si>
-    <t>sales-free-get-ms</t>
-  </si>
-  <si>
-    <t>sales-opt-get-ms</t>
-  </si>
-  <si>
     <t>sale-delete-ms</t>
   </si>
   <si>
@@ -224,21 +212,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>sale-save-ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /selling/data/get/opt/sale/v1/</t>
-  </si>
-  <si>
-    <t>/selling/data/manager/sale/v1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /selling/data/get/free/sale/v1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /selling/data/save/sale/v1/</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /selling/data/delete/sale/v1/</t>
   </si>
   <si>
@@ -254,36 +227,15 @@
     <t xml:space="preserve"> /selling/data/update/sales/v1/</t>
   </si>
   <si>
-    <t>/selling/data/get/manager/sale/v1/</t>
-  </si>
-  <si>
-    <t>/selling/data/save/manager/sale/v1/</t>
-  </si>
-  <si>
     <t>/selling/data/delete/manager/sale/v1/</t>
   </si>
   <si>
     <t>/selling/data/update/manager/sale/v1/</t>
   </si>
   <si>
-    <t xml:space="preserve"> /selling/data/get/query/sale/v1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /selling/data/save/sales/v1/</t>
-  </si>
-  <si>
     <t>kafka-sale-consumer-ms</t>
   </si>
   <si>
-    <t>data-manager-ms</t>
-  </si>
-  <si>
-    <t>data-get-manager-ms</t>
-  </si>
-  <si>
-    <t>data-save-manager-ms</t>
-  </si>
-  <si>
     <t>data-delete-manager-ms</t>
   </si>
   <si>
@@ -429,14 +381,70 @@
   </si>
   <si>
     <t>redis-insight</t>
+  </si>
+  <si>
+    <t>/orderizer/data/get/search/orders/v1/</t>
+  </si>
+  <si>
+    <t>data-get-search-orders</t>
+  </si>
+  <si>
+    <t>data-get-free-orders</t>
+  </si>
+  <si>
+    <t>data-get-opt-orders</t>
+  </si>
+  <si>
+    <t>/orderizer/data/get/free/orders/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/data/get/opt/orders/v1/</t>
+  </si>
+  <si>
+    <t>data-save-order</t>
+  </si>
+  <si>
+    <t>data-save-orders</t>
+  </si>
+  <si>
+    <t>data-save-orders-manager</t>
+  </si>
+  <si>
+    <t>data-get-orders-manager</t>
+  </si>
+  <si>
+    <t>/orderizer/data/get/orders/manager/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/data/orders/manager/v1/</t>
+  </si>
+  <si>
+    <t>data-orders-manager</t>
+  </si>
+  <si>
+    <t>/orderizer/data/save/orders/manager/v1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /orderizer/data/save/order/v1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /orderizer/data/save/orders/v1/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -527,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -554,6 +562,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -872,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D46" sqref="C46:D50"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,7 +900,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -906,16 +920,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D2" s="8">
         <v>6010</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -957,7 +971,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -966,7 +980,7 @@
         <v>6040</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -974,16 +988,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D6" s="4">
         <v>6041</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -994,13 +1008,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1">
         <v>6060</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1021,139 +1035,139 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="11">
         <v>11</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="B9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="11">
         <v>6080</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>64</v>
+      <c r="E9" s="11" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="A10" s="10">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="10">
         <v>6081</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>72</v>
+      <c r="E10" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="A11" s="10">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="B11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="10">
         <v>6082</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>76</v>
+      <c r="E11" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="A12" s="10">
         <v>14</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="7">
+      <c r="C12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="10">
         <v>6083</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>65</v>
+      <c r="E12" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="A13" s="10">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="B13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="10">
         <v>6084</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>63</v>
+      <c r="E13" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="11">
         <v>16</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="5">
+      <c r="B14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="11">
         <v>6085</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>73</v>
+      <c r="E14" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="11">
         <v>17</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="5">
+      <c r="B15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="11">
         <v>6086</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>66</v>
+      <c r="E15" s="11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16" s="11">
         <v>18</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="5">
+      <c r="B16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="11">
         <v>6087</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>77</v>
+      <c r="E16" s="11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1161,16 +1175,16 @@
         <v>19</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D17" s="7">
         <v>6088</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1178,16 +1192,16 @@
         <v>20</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D18" s="7">
         <v>6089</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1195,16 +1209,16 @@
         <v>21</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D19" s="7">
         <v>6090</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1212,16 +1226,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D20" s="7">
         <v>6091</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1229,16 +1243,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D21" s="5">
         <v>6092</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1246,16 +1260,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D22" s="5">
         <v>6093</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1263,16 +1277,16 @@
         <v>25</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" s="5">
         <v>6094</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1280,16 +1294,16 @@
         <v>26</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D24" s="6">
         <v>7000</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1297,16 +1311,16 @@
         <v>27</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="D25" s="6">
         <v>7001</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1314,16 +1328,16 @@
         <v>28</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D26" s="6">
         <v>7002</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1331,16 +1345,16 @@
         <v>29</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D27" s="6">
         <v>7003</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1348,16 +1362,16 @@
         <v>30</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D28" s="6">
         <v>7004</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1365,16 +1379,16 @@
         <v>31</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" s="6">
         <v>7005</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1382,16 +1396,16 @@
         <v>32</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" s="6">
         <v>7006</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1399,16 +1413,16 @@
         <v>33</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D31" s="6">
         <v>7007</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1416,16 +1430,16 @@
         <v>34</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D32" s="6">
         <v>7008</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1433,16 +1447,16 @@
         <v>35</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D33" s="6">
         <v>7009</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1450,16 +1464,16 @@
         <v>36</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D34" s="6">
         <v>7010</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1467,16 +1481,16 @@
         <v>37</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D35" s="6">
         <v>7011</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1484,16 +1498,16 @@
         <v>38</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D36" s="6">
         <v>7012</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1501,16 +1515,16 @@
         <v>39</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D37" s="6">
         <v>7013</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1518,16 +1532,16 @@
         <v>40</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D38" s="6">
         <v>7014</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1535,16 +1549,16 @@
         <v>41</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D39" s="6">
         <v>7015</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1552,16 +1566,16 @@
         <v>42</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D40" s="6">
         <v>7016</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1569,16 +1583,16 @@
         <v>43</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D41" s="6">
         <v>7017</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1586,16 +1600,16 @@
         <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1">
         <v>7020</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1603,16 +1617,16 @@
         <v>45</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1">
         <v>7021</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1620,16 +1634,16 @@
         <v>46</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D44" s="1">
         <v>7022</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1637,16 +1651,16 @@
         <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D45" s="1">
         <v>7023</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1654,16 +1668,16 @@
         <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D46" s="3">
         <v>7030</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1671,16 +1685,16 @@
         <v>49</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D47" s="3">
         <v>7031</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1688,16 +1702,16 @@
         <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D48" s="3">
         <v>7032</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1705,16 +1719,16 @@
         <v>51</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D49" s="3">
         <v>7033</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1722,16 +1736,16 @@
         <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D50" s="3">
         <v>7034</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1739,16 +1753,16 @@
         <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D51" s="3">
         <v>7035</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1756,16 +1770,16 @@
         <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="D52" s="5">
         <v>7040</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1773,16 +1787,16 @@
         <v>55</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D53" s="5">
         <v>7041</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1790,16 +1804,16 @@
         <v>56</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="D54" s="5">
         <v>7042</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1807,16 +1821,16 @@
         <v>57</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D55" s="5">
         <v>7043</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1824,16 +1838,16 @@
         <v>58</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="D56" s="9">
         <v>7050</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1841,16 +1855,16 @@
         <v>59</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="D57" s="9">
         <v>7051</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1858,16 +1872,16 @@
         <v>60</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="D58" s="9">
         <v>7052</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1875,16 +1889,16 @@
         <v>61</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D59" s="9">
         <v>7053</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1892,16 +1906,16 @@
         <v>62</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D60" s="9">
         <v>7054</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1909,16 +1923,16 @@
         <v>63</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D61" s="9">
         <v>7055</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1926,16 +1940,16 @@
         <v>64</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="D62" s="9">
         <v>7056</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1943,16 +1957,16 @@
         <v>65</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D63" s="9">
         <v>7057</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DEV: Change the project names of data/delete category.
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF3705C-686F-4E43-86FB-FD48A47E4F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB18B4D4-0332-8344-9CB1-38AC1B969EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t xml:space="preserve"> /selling/source/push/sale/v1/</t>
   </si>
   <si>
-    <t>sales-delete-ms</t>
-  </si>
-  <si>
     <t>sales-update-ms</t>
   </si>
   <si>
@@ -203,48 +200,27 @@
     <t>search-sales-manager-ms</t>
   </si>
   <si>
-    <t>sale-delete-ms</t>
-  </si>
-  <si>
     <t>sale-update-ms</t>
   </si>
   <si>
     <t>data</t>
   </si>
   <si>
-    <t xml:space="preserve"> /selling/data/delete/sale/v1/</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /selling/data/update/sale/v1/</t>
   </si>
   <si>
-    <t xml:space="preserve"> /selling/data/delete/sales/v1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /selling/data/delete/query/sales/v1/</t>
-  </si>
-  <si>
     <t xml:space="preserve"> /selling/data/update/sales/v1/</t>
   </si>
   <si>
-    <t>/selling/data/delete/manager/sale/v1/</t>
-  </si>
-  <si>
     <t>/selling/data/update/manager/sale/v1/</t>
   </si>
   <si>
     <t>kafka-sale-consumer-ms</t>
   </si>
   <si>
-    <t>data-delete-manager-ms</t>
-  </si>
-  <si>
     <t>data-update-manager-ms</t>
   </si>
   <si>
-    <t>sales-delete-query-ms</t>
-  </si>
-  <si>
     <t>shared</t>
   </si>
   <si>
@@ -429,6 +405,30 @@
   </si>
   <si>
     <t xml:space="preserve"> /orderizer/data/save/orders/v1/</t>
+  </si>
+  <si>
+    <t>data-delete-orders-manager</t>
+  </si>
+  <si>
+    <t>data-delete-order</t>
+  </si>
+  <si>
+    <t>data-delete-orders</t>
+  </si>
+  <si>
+    <t>data-delete-search-orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /orderizer/data/delete/order/v1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /orderizer/data/delete/orders/v1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /orderizer/data/delete/search/orders/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/data/delete/orders/manager/v1/</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,7 +900,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -920,16 +920,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D2" s="8">
         <v>6010</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -971,7 +971,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -980,7 +980,7 @@
         <v>6040</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -988,16 +988,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D6" s="4">
         <v>6041</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1008,13 +1008,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1">
         <v>6060</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1039,16 +1039,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D9" s="11">
         <v>6080</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1056,16 +1056,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D10" s="10">
         <v>6081</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1073,16 +1073,16 @@
         <v>13</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D11" s="10">
         <v>6082</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1090,16 +1090,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D12" s="10">
         <v>6083</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1107,67 +1107,67 @@
         <v>15</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D13" s="10">
         <v>6084</v>
       </c>
       <c r="E13" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6085</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="11">
-        <v>16</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="11">
-        <v>6085</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="11">
+      <c r="A15" s="5">
         <v>17</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6086</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="11">
-        <v>6086</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="11">
+      <c r="A16" s="5">
         <v>18</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="5">
+        <v>6087</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="D16" s="11">
-        <v>6087</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1175,16 +1175,16 @@
         <v>19</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="D17" s="7">
         <v>6088</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1192,16 +1192,16 @@
         <v>20</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="D18" s="7">
         <v>6089</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1209,16 +1209,16 @@
         <v>21</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="D19" s="7">
         <v>6090</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1226,16 +1226,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="D20" s="7">
         <v>6091</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>61</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1243,16 +1243,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D21" s="5">
         <v>6092</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1260,16 +1260,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="5">
         <v>6093</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1277,16 +1277,16 @@
         <v>25</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="5">
         <v>6094</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1294,16 +1294,16 @@
         <v>26</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="6">
         <v>7000</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1311,16 +1311,16 @@
         <v>27</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="6">
         <v>7001</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1328,16 +1328,16 @@
         <v>28</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="6">
         <v>7002</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1345,16 +1345,16 @@
         <v>29</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" s="6">
         <v>7003</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,16 +1362,16 @@
         <v>30</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" s="6">
         <v>7004</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1379,16 +1379,16 @@
         <v>31</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29" s="6">
         <v>7005</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1396,16 +1396,16 @@
         <v>32</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" s="6">
         <v>7006</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1413,16 +1413,16 @@
         <v>33</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" s="6">
         <v>7007</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1430,16 +1430,16 @@
         <v>34</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" s="6">
         <v>7008</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1447,16 +1447,16 @@
         <v>35</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" s="6">
         <v>7009</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1464,16 +1464,16 @@
         <v>36</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="6">
         <v>7010</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1481,16 +1481,16 @@
         <v>37</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="6">
         <v>7011</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1498,16 +1498,16 @@
         <v>38</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D36" s="6">
         <v>7012</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1515,16 +1515,16 @@
         <v>39</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" s="6">
         <v>7013</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1532,16 +1532,16 @@
         <v>40</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="6">
         <v>7014</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1549,16 +1549,16 @@
         <v>41</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" s="6">
         <v>7015</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1566,16 +1566,16 @@
         <v>42</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" s="6">
         <v>7016</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1583,16 +1583,16 @@
         <v>43</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="6">
         <v>7017</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1600,16 +1600,16 @@
         <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D42" s="1">
         <v>7020</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1617,16 +1617,16 @@
         <v>45</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D43" s="1">
         <v>7021</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1634,16 +1634,16 @@
         <v>46</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D44" s="1">
         <v>7022</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1651,16 +1651,16 @@
         <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D45" s="1">
         <v>7023</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1668,16 +1668,16 @@
         <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D46" s="3">
         <v>7030</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1685,16 +1685,16 @@
         <v>49</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D47" s="3">
         <v>7031</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1702,16 +1702,16 @@
         <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D48" s="3">
         <v>7032</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1719,16 +1719,16 @@
         <v>51</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D49" s="3">
         <v>7033</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1736,16 +1736,16 @@
         <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D50" s="3">
         <v>7034</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1753,16 +1753,16 @@
         <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D51" s="3">
         <v>7035</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1770,16 +1770,16 @@
         <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D52" s="5">
         <v>7040</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1787,16 +1787,16 @@
         <v>55</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D53" s="5">
         <v>7041</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1804,16 +1804,16 @@
         <v>56</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D54" s="5">
         <v>7042</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1821,16 +1821,16 @@
         <v>57</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D55" s="5">
         <v>7043</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1838,16 +1838,16 @@
         <v>58</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D56" s="9">
         <v>7050</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1855,16 +1855,16 @@
         <v>59</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D57" s="9">
         <v>7051</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1872,16 +1872,16 @@
         <v>60</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D58" s="9">
         <v>7052</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1889,16 +1889,16 @@
         <v>61</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D59" s="9">
         <v>7053</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1906,16 +1906,16 @@
         <v>62</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D60" s="9">
         <v>7054</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1923,16 +1923,16 @@
         <v>63</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D61" s="9">
         <v>7055</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1940,16 +1940,16 @@
         <v>64</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D62" s="9">
         <v>7056</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1957,16 +1957,16 @@
         <v>65</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D63" s="9">
         <v>7057</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DEV: change the docker related files after refactoring the delete category
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB18B4D4-0332-8344-9CB1-38AC1B969EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AC4D82-B919-174F-B557-44AFC45CA255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="130">
   <si>
     <t>service-name</t>
   </si>
@@ -77,9 +77,6 @@
     <t xml:space="preserve"> /selling/source/push/sale/v1/</t>
   </si>
   <si>
-    <t>sales-update-ms</t>
-  </si>
-  <si>
     <t>kafka</t>
   </si>
   <si>
@@ -200,27 +197,12 @@
     <t>search-sales-manager-ms</t>
   </si>
   <si>
-    <t>sale-update-ms</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
-    <t xml:space="preserve"> /selling/data/update/sale/v1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /selling/data/update/sales/v1/</t>
-  </si>
-  <si>
-    <t>/selling/data/update/manager/sale/v1/</t>
-  </si>
-  <si>
     <t>kafka-sale-consumer-ms</t>
   </si>
   <si>
-    <t>data-update-manager-ms</t>
-  </si>
-  <si>
     <t>shared</t>
   </si>
   <si>
@@ -429,22 +411,29 @@
   </si>
   <si>
     <t>/orderizer/data/delete/orders/manager/v1/</t>
+  </si>
+  <si>
+    <t>data-update-orders-manager</t>
+  </si>
+  <si>
+    <t>data-update-order</t>
+  </si>
+  <si>
+    <t>data-update-orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /orderizer/data/update/order/v1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /orderizer/data/update/orders/v1/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -564,10 +553,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -887,7 +876,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,7 +889,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -920,16 +909,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D2" s="8">
         <v>6010</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -971,7 +960,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -980,7 +969,7 @@
         <v>6040</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -988,16 +977,16 @@
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D6" s="4">
         <v>6041</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1008,13 +997,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1">
         <v>6060</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1035,88 +1024,88 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>11</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="B9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="10">
         <v>6080</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>118</v>
+      <c r="E9" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="11">
         <v>12</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="B10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="11">
         <v>6081</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>117</v>
+      <c r="E10" s="11" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+      <c r="A11" s="11">
         <v>13</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="B11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="11">
         <v>6082</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>107</v>
+      <c r="E11" s="11" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+      <c r="A12" s="11">
         <v>14</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="B12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="11">
         <v>6083</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>111</v>
+      <c r="E12" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="10">
+      <c r="A13" s="11">
         <v>15</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="B13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="11">
         <v>6084</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>112</v>
+      <c r="E13" s="11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1124,16 +1113,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D14" s="5">
         <v>6085</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1141,16 +1130,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D15" s="5">
         <v>6086</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1158,16 +1147,16 @@
         <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D16" s="5">
         <v>6087</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1175,16 +1164,16 @@
         <v>19</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D17" s="7">
         <v>6088</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1192,16 +1181,16 @@
         <v>20</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D18" s="7">
         <v>6089</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1209,16 +1198,16 @@
         <v>21</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D19" s="7">
         <v>6090</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1226,16 +1215,16 @@
         <v>22</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D20" s="7">
         <v>6091</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1243,16 +1232,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="D21" s="5">
         <v>6092</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1260,16 +1249,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="D22" s="5">
         <v>6093</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1277,16 +1266,16 @@
         <v>25</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="D23" s="5">
         <v>6094</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1294,16 +1283,16 @@
         <v>26</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="6">
         <v>7000</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1311,16 +1300,16 @@
         <v>27</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="6">
         <v>7001</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1328,16 +1317,16 @@
         <v>28</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="6">
         <v>7002</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1345,16 +1334,16 @@
         <v>29</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="6">
         <v>7003</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,16 +1351,16 @@
         <v>30</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="6">
         <v>7004</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1379,16 +1368,16 @@
         <v>31</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="6">
         <v>7005</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1396,16 +1385,16 @@
         <v>32</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="6">
         <v>7006</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1413,16 +1402,16 @@
         <v>33</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="6">
         <v>7007</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1430,16 +1419,16 @@
         <v>34</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="6">
         <v>7008</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1447,16 +1436,16 @@
         <v>35</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="6">
         <v>7009</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1464,16 +1453,16 @@
         <v>36</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="6">
         <v>7010</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1481,16 +1470,16 @@
         <v>37</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="6">
         <v>7011</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1498,16 +1487,16 @@
         <v>38</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="6">
         <v>7012</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1515,16 +1504,16 @@
         <v>39</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="6">
         <v>7013</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1532,16 +1521,16 @@
         <v>40</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D38" s="6">
         <v>7014</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1549,16 +1538,16 @@
         <v>41</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" s="6">
         <v>7015</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1566,16 +1555,16 @@
         <v>42</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="6">
         <v>7016</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1583,16 +1572,16 @@
         <v>43</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D41" s="6">
         <v>7017</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1600,16 +1589,16 @@
         <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D42" s="1">
         <v>7020</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1617,16 +1606,16 @@
         <v>45</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D43" s="1">
         <v>7021</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1634,16 +1623,16 @@
         <v>46</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D44" s="1">
         <v>7022</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1651,16 +1640,16 @@
         <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D45" s="1">
         <v>7023</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1668,16 +1657,16 @@
         <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D46" s="3">
         <v>7030</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1685,16 +1674,16 @@
         <v>49</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D47" s="3">
         <v>7031</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1702,16 +1691,16 @@
         <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D48" s="3">
         <v>7032</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1719,16 +1708,16 @@
         <v>51</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D49" s="3">
         <v>7033</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1736,16 +1725,16 @@
         <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D50" s="3">
         <v>7034</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1753,16 +1742,16 @@
         <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D51" s="3">
         <v>7035</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1770,16 +1759,16 @@
         <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D52" s="5">
         <v>7040</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1787,16 +1776,16 @@
         <v>55</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D53" s="5">
         <v>7041</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1804,16 +1793,16 @@
         <v>56</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D54" s="5">
         <v>7042</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1821,16 +1810,16 @@
         <v>57</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D55" s="5">
         <v>7043</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1838,16 +1827,16 @@
         <v>58</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D56" s="9">
         <v>7050</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1855,16 +1844,16 @@
         <v>59</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D57" s="9">
         <v>7051</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1872,16 +1861,16 @@
         <v>60</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D58" s="9">
         <v>7052</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1889,16 +1878,16 @@
         <v>61</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D59" s="9">
         <v>7053</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1906,16 +1895,16 @@
         <v>62</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D60" s="9">
         <v>7054</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1923,16 +1912,16 @@
         <v>63</v>
       </c>
       <c r="B61" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="D61" s="9">
         <v>7055</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1940,16 +1929,16 @@
         <v>64</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D62" s="9">
         <v>7056</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1957,16 +1946,16 @@
         <v>65</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D63" s="9">
         <v>7057</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DEV: Change the names of update category
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AC4D82-B919-174F-B557-44AFC45CA255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D300476A-2101-534A-8E09-3F181CE83BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,10 +422,10 @@
     <t>data-update-orders</t>
   </si>
   <si>
-    <t xml:space="preserve"> /orderizer/data/update/order/v1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /orderizer/data/update/orders/v1/</t>
+    <t>/orderizer/data/update/order/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/data/update/orders/v1/</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -551,12 +551,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -876,7 +870,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,87 +1018,87 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="A9" s="5">
         <v>11</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="5">
         <v>6080</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="11">
+      <c r="A10" s="7">
         <v>12</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="7">
         <v>6081</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
+      <c r="A11" s="7">
         <v>13</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="7">
         <v>6082</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="7" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
+      <c r="A12" s="7">
         <v>14</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="7">
         <v>6083</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="11">
+      <c r="A13" s="7">
         <v>15</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="7">
         <v>6084</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="7" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DEV: Refactor the data-update-orders service
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Selling-System/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C381003-A308-7F4B-B533-F62EDE6D8F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2A574E-B975-FD41-8151-8C779B0F98F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -753,7 +753,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E5" sqref="C5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DEV: Remove the main class from the core.
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Orderizer/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C96DAF-578F-B746-A055-D3DC7B10282E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61CC42C-71EE-294B-8B57-C6AC88B2CD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -675,7 +675,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DEV: Start refactoring export category
</commit_message>
<xml_diff>
--- a/docs/configuration/services-details.xlsx
+++ b/docs/configuration/services-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdfrehat/Frehat/Code/Projects/Orderizer/docs/configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61CC42C-71EE-294B-8B57-C6AC88B2CD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A0229-F833-E24D-AA4A-FFADBC1FA0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{3A3E2F0A-FFA9-424C-A817-011C25B3DD11}"/>
   </bookViews>
@@ -200,42 +200,6 @@
     <t>/orderizer/modify/v1/</t>
   </si>
   <si>
-    <t>/orderizer/export/manager/</t>
-  </si>
-  <si>
-    <t>/orderizer/export/orders/pdf/</t>
-  </si>
-  <si>
-    <t>/orderizer/export/orders/csv/</t>
-  </si>
-  <si>
-    <t>/orderizer/export/orders/xlsx/</t>
-  </si>
-  <si>
-    <t>/orderizer/export/orders/json/</t>
-  </si>
-  <si>
-    <t>/orderizer/export/orders/xml/</t>
-  </si>
-  <si>
-    <t>export-data-orders-pdf</t>
-  </si>
-  <si>
-    <t>export-data-orders-csv</t>
-  </si>
-  <si>
-    <t>export-data-orders-xlsx</t>
-  </si>
-  <si>
-    <t>export-data-orders-json</t>
-  </si>
-  <si>
-    <t>export-data-orders-xml</t>
-  </si>
-  <si>
-    <t>export-manager</t>
-  </si>
-  <si>
     <t>/orderizer/kafka/orders/consumer</t>
   </si>
   <si>
@@ -258,6 +222,42 @@
   </si>
   <si>
     <t>report</t>
+  </si>
+  <si>
+    <t>export-data-json</t>
+  </si>
+  <si>
+    <t>export-data-xlsx</t>
+  </si>
+  <si>
+    <t>export-data-csv</t>
+  </si>
+  <si>
+    <t>export-data-pdf</t>
+  </si>
+  <si>
+    <t>export-data-xml</t>
+  </si>
+  <si>
+    <t>/orderizer/export/data/pdf/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/export/data/csv/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/export/data/xlsx/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/export/data/json/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/export/data/xml/v1/</t>
+  </si>
+  <si>
+    <t>/orderizer/export/data/manager/v1/</t>
+  </si>
+  <si>
+    <t>export-data-manager</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6570D666-0A27-C04A-A7C2-ED7EE227A969}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,10 +708,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3">
         <v>6020</v>
@@ -728,13 +728,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D3" s="4">
         <v>6040</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -745,13 +745,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D4" s="4">
         <v>6041</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1">
         <v>6060</v>
@@ -779,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1">
         <v>6061</v>
@@ -1068,13 +1068,13 @@
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D23" s="3">
         <v>7030</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1085,13 +1085,13 @@
         <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D24" s="3">
         <v>7031</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1102,13 +1102,13 @@
         <v>10</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3">
         <v>7032</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1119,13 +1119,13 @@
         <v>10</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" s="3">
         <v>7033</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1136,13 +1136,13 @@
         <v>10</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D27" s="3">
         <v>7034</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1153,13 +1153,13 @@
         <v>10</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D28" s="3">
         <v>7035</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>